<commit_message>
nome arquivo FOrm161 corrigido
</commit_message>
<xml_diff>
--- a/Forms/Form_161_Gerado/2023/Março/08.03/08.03.2023_16.51.xlsx
+++ b/Forms/Form_161_Gerado/2023/Março/08.03/08.03.2023_16.51.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levym\OneDrive\Documentos\Projects\Tecplas\Sis-Pint\projeto_pintura\Forms\Form_161_Gerado\2023\Março\08.03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8772B98-CB18-4E4E-A3AB-DF75A071CDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B17DA28-2A5F-4F44-84EC-C78661CE4573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="F966" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_FilterDatabase" localSheetId="1" hidden="1">Dados!$A$1:$L$69</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Planilha1!$A$1:$K$56</definedName>
     <definedName name="Print_Area" localSheetId="2">'40-157'!$B$1:$L$59</definedName>
     <definedName name="Print_Area" localSheetId="0">Planilha1!$A$1:$K$56</definedName>
   </definedNames>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="239">
   <si>
     <t>Descrições de parâmetros/ controles</t>
   </si>
@@ -743,9 +744,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                 </t>
   </si>
   <si>
     <t>TINTA POLIURETANO SEMI BRILHO CINZA</t>
@@ -1798,80 +1796,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1885,49 +1856,16 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1984,6 +1922,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1993,152 +1937,206 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9722,10 +9720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O99"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A30" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:E49"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A38" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9739,78 +9737,70 @@
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="21.33203125" customWidth="1"/>
     <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="133" t="s">
+    <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="113" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="135"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="136"/>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="138"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="141" t="s">
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="115"/>
+    </row>
+    <row r="2" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="116"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="118"/>
+    </row>
+    <row r="3" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="121" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="142"/>
-      <c r="C3" s="144" t="s">
+      <c r="B3" s="122"/>
+      <c r="C3" s="124" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="119">
+        <v>1452803</v>
+      </c>
+      <c r="K3" s="120"/>
+    </row>
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="121" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="122"/>
+      <c r="C4" s="125" t="s">
         <v>238</v>
       </c>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="142"/>
-      <c r="J3" s="139">
-        <v>1452803</v>
-      </c>
-      <c r="K3" s="140"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="141" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="142"/>
-      <c r="C4" s="145" t="s">
-        <v>239</v>
-      </c>
-      <c r="D4" s="145"/>
-      <c r="E4" s="145"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="147" t="s">
+      <c r="D4" s="125"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="148"/>
+      <c r="H4" s="128"/>
       <c r="I4" s="83">
         <v>44993</v>
       </c>
@@ -9819,66 +9809,66 @@
         <v>2441</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="113" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="113"/>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="113"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="113"/>
-      <c r="B7" s="113"/>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="113"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="113"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="107" t="s">
+      <c r="B6" s="129"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="129"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="129"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="129"/>
+      <c r="H7" s="129"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="129"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="168" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="107"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="107"/>
-      <c r="G8" s="107"/>
-      <c r="H8" s="97" t="s">
+      <c r="B8" s="168"/>
+      <c r="C8" s="168"/>
+      <c r="D8" s="168"/>
+      <c r="E8" s="168"/>
+      <c r="F8" s="168"/>
+      <c r="G8" s="168"/>
+      <c r="H8" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="97"/>
-      <c r="J8" s="97" t="s">
+      <c r="I8" s="100"/>
+      <c r="J8" s="100" t="s">
         <v>123</v>
       </c>
-      <c r="K8" s="97"/>
-    </row>
-    <row r="9" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="107"/>
-      <c r="B9" s="107"/>
-      <c r="C9" s="107"/>
-      <c r="D9" s="107"/>
-      <c r="E9" s="107"/>
-      <c r="F9" s="107"/>
-      <c r="G9" s="107"/>
+      <c r="K8" s="100"/>
+    </row>
+    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="168"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="168"/>
+      <c r="D9" s="168"/>
+      <c r="E9" s="168"/>
+      <c r="F9" s="168"/>
+      <c r="G9" s="168"/>
       <c r="H9" s="4" t="s">
         <v>18</v>
       </c>
@@ -9887,18 +9877,15 @@
         <v>18</v>
       </c>
       <c r="K9" s="80"/>
-      <c r="M9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="107"/>
-      <c r="B10" s="107"/>
-      <c r="C10" s="107"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="107"/>
-      <c r="G10" s="107"/>
+    </row>
+    <row r="10" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="168"/>
+      <c r="B10" s="168"/>
+      <c r="C10" s="168"/>
+      <c r="D10" s="168"/>
+      <c r="E10" s="168"/>
+      <c r="F10" s="168"/>
+      <c r="G10" s="168"/>
       <c r="H10" s="4" t="s">
         <v>17</v>
       </c>
@@ -9908,14 +9895,14 @@
       </c>
       <c r="K10" s="80"/>
     </row>
-    <row r="11" spans="1:13" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="107"/>
-      <c r="B11" s="107"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="107"/>
+    <row r="11" spans="1:11" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="168"/>
+      <c r="B11" s="168"/>
+      <c r="C11" s="168"/>
+      <c r="D11" s="168"/>
+      <c r="E11" s="168"/>
+      <c r="F11" s="168"/>
+      <c r="G11" s="168"/>
       <c r="H11" s="4" t="s">
         <v>106</v>
       </c>
@@ -9929,14 +9916,14 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="107"/>
-      <c r="B12" s="107"/>
-      <c r="C12" s="107"/>
-      <c r="D12" s="107"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
-      <c r="G12" s="107"/>
+    <row r="12" spans="1:11" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="168"/>
+      <c r="B12" s="168"/>
+      <c r="C12" s="168"/>
+      <c r="D12" s="168"/>
+      <c r="E12" s="168"/>
+      <c r="F12" s="168"/>
+      <c r="G12" s="168"/>
       <c r="H12" s="4" t="s">
         <v>107</v>
       </c>
@@ -9950,7 +9937,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -9963,51 +9950,51 @@
       <c r="J13" s="11"/>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="98" t="s">
+    <row r="14" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="161" t="s">
         <v>110</v>
       </c>
-      <c r="B14" s="99"/>
-      <c r="C14" s="99"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="101" t="str">
+      <c r="B14" s="162"/>
+      <c r="C14" s="162"/>
+      <c r="D14" s="163"/>
+      <c r="E14" s="134" t="str">
         <f>VLOOKUP(J3,Dados!A:H,5,0)</f>
         <v>35 a 50psi</v>
       </c>
-      <c r="F14" s="102"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="108" t="s">
+      <c r="F14" s="164"/>
+      <c r="G14" s="135"/>
+      <c r="H14" s="130" t="s">
         <v>121</v>
       </c>
-      <c r="I14" s="108"/>
-      <c r="J14" s="108" t="s">
+      <c r="I14" s="130"/>
+      <c r="J14" s="130" t="s">
         <v>122</v>
       </c>
-      <c r="K14" s="108"/>
-    </row>
-    <row r="15" spans="1:13" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="98" t="s">
+      <c r="K14" s="130"/>
+    </row>
+    <row r="15" spans="1:11" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="161" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="99"/>
-      <c r="C15" s="99"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="99"/>
-      <c r="F15" s="99"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="99"/>
-      <c r="J15" s="99"/>
-      <c r="K15" s="100"/>
-    </row>
-    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="104"/>
-      <c r="B16" s="105"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="106"/>
+      <c r="B15" s="162"/>
+      <c r="C15" s="162"/>
+      <c r="D15" s="162"/>
+      <c r="E15" s="162"/>
+      <c r="F15" s="162"/>
+      <c r="G15" s="162"/>
+      <c r="H15" s="162"/>
+      <c r="I15" s="162"/>
+      <c r="J15" s="162"/>
+      <c r="K15" s="163"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="165"/>
+      <c r="B16" s="166"/>
+      <c r="C16" s="166"/>
+      <c r="D16" s="166"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="167"/>
       <c r="H16" s="26" t="s">
         <v>2</v>
       </c>
@@ -10021,16 +10008,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="149"/>
-      <c r="B17" s="150"/>
-      <c r="C17" s="150"/>
-      <c r="D17" s="150"/>
-      <c r="E17" s="151"/>
-      <c r="F17" s="132" t="s">
+    <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="131"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="132"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="112" t="s">
         <v>125</v>
       </c>
-      <c r="G17" s="132"/>
+      <c r="G17" s="112"/>
       <c r="H17" s="29" t="str">
         <f>VLOOKUP(J3,Dados!A:N,14,0)</f>
         <v>____:____</v>
@@ -10048,26 +10035,26 @@
         <v>____:____</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="B18" s="101" t="str">
+      <c r="B18" s="134" t="str">
         <f>VLOOKUP(J3,Dados!A:W,23,0)</f>
         <v>1.2 a 1.4</v>
       </c>
-      <c r="C18" s="103"/>
-      <c r="D18" s="164" t="s">
+      <c r="C18" s="135"/>
+      <c r="D18" s="103" t="s">
         <v>147</v>
       </c>
-      <c r="E18" s="164" t="str">
+      <c r="E18" s="103" t="str">
         <f>VLOOKUP(J3,Dados!A:M,13,0)</f>
         <v>N/A</v>
       </c>
-      <c r="F18" s="97" t="s">
+      <c r="F18" s="100" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="97"/>
+      <c r="G18" s="100"/>
       <c r="H18" s="2" t="str">
         <f>VLOOKUP(J3,Dados!A:P,16,0)</f>
         <v>N/A</v>
@@ -10085,21 +10072,21 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="162" t="s">
+    <row r="19" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="101" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="97">
+      <c r="B19" s="100">
         <f>VLOOKUP(J3,Dados!A:L,12,0)</f>
         <v>1</v>
       </c>
-      <c r="C19" s="97"/>
-      <c r="D19" s="165"/>
-      <c r="E19" s="165"/>
-      <c r="F19" s="97" t="s">
-        <v>229</v>
-      </c>
-      <c r="G19" s="97"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="100" t="s">
+        <v>228</v>
+      </c>
+      <c r="G19" s="100"/>
       <c r="H19" s="2" t="str">
         <f>VLOOKUP(J3,Dados!A:R,18,0)</f>
         <v>N/A</v>
@@ -10117,16 +10104,16 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="163"/>
-      <c r="B20" s="161"/>
-      <c r="C20" s="161"/>
-      <c r="D20" s="166"/>
-      <c r="E20" s="166"/>
-      <c r="F20" s="161" t="s">
+    <row r="20" spans="1:11" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="102"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="99" t="s">
         <v>133</v>
       </c>
-      <c r="G20" s="161"/>
+      <c r="G20" s="99"/>
       <c r="H20" s="32" t="str">
         <f>VLOOKUP(J3,Dados!A:T,20,0)</f>
         <v>N/A</v>
@@ -10144,160 +10131,158 @@
         <v>N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="93" t="s">
+    <row r="21" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="157" t="s">
         <v>111</v>
       </c>
-      <c r="B21" s="94"/>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="102" t="str">
+      <c r="B21" s="158"/>
+      <c r="C21" s="158"/>
+      <c r="D21" s="158"/>
+      <c r="E21" s="164" t="str">
         <f>VLOOKUP(J3,Dados!A1:F75,6,0)</f>
         <v>N/A</v>
       </c>
-      <c r="F21" s="102"/>
-      <c r="G21" s="103"/>
+      <c r="F21" s="164"/>
+      <c r="G21" s="135"/>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
       <c r="J21" s="27"/>
       <c r="K21" s="28"/>
     </row>
-    <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="98" t="s">
+    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="161" t="s">
         <v>112</v>
       </c>
-      <c r="B22" s="99"/>
-      <c r="C22" s="99"/>
-      <c r="D22" s="99"/>
-      <c r="E22" s="102" t="str">
+      <c r="B22" s="162"/>
+      <c r="C22" s="162"/>
+      <c r="D22" s="162"/>
+      <c r="E22" s="164" t="str">
         <f>VLOOKUP(J3,Dados!A:H,8,0)</f>
         <v>120 min./ Mínimo</v>
       </c>
-      <c r="F22" s="102"/>
-      <c r="G22" s="103"/>
+      <c r="F22" s="164"/>
+      <c r="G22" s="135"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="98" t="s">
+    <row r="23" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="161" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="99"/>
-      <c r="C23" s="99"/>
-      <c r="D23" s="99"/>
-      <c r="E23" s="102" t="str">
+      <c r="B23" s="162"/>
+      <c r="C23" s="162"/>
+      <c r="D23" s="162"/>
+      <c r="E23" s="164" t="str">
         <f>VLOOKUP(J3,Dados!A:H,7,0)</f>
         <v>25°C +/- 2°C</v>
       </c>
-      <c r="F23" s="102"/>
-      <c r="G23" s="103"/>
-      <c r="H23" s="95"/>
-      <c r="I23" s="95"/>
-      <c r="J23" s="96"/>
-      <c r="K23" s="96"/>
-    </row>
-    <row r="24" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="109" t="s">
+      <c r="F23" s="164"/>
+      <c r="G23" s="135"/>
+      <c r="H23" s="159"/>
+      <c r="I23" s="159"/>
+      <c r="J23" s="160"/>
+      <c r="K23" s="160"/>
+    </row>
+    <row r="24" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="136" t="s">
         <v>119</v>
       </c>
-      <c r="B25" s="110"/>
-      <c r="C25" s="110"/>
-      <c r="D25" s="110"/>
-      <c r="E25" s="110"/>
-      <c r="F25" s="110"/>
-      <c r="G25" s="110"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="110"/>
-      <c r="J25" s="110"/>
-      <c r="K25" s="111"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="112"/>
-      <c r="B26" s="113"/>
-      <c r="C26" s="113"/>
-      <c r="D26" s="113"/>
-      <c r="E26" s="113"/>
-      <c r="F26" s="113"/>
-      <c r="G26" s="113"/>
-      <c r="H26" s="113"/>
-      <c r="I26" s="113"/>
-      <c r="J26" s="113"/>
-      <c r="K26" s="114"/>
-    </row>
-    <row r="27" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="121" t="s">
+      <c r="B25" s="137"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="137"/>
+      <c r="E25" s="137"/>
+      <c r="F25" s="137"/>
+      <c r="G25" s="137"/>
+      <c r="H25" s="137"/>
+      <c r="I25" s="137"/>
+      <c r="J25" s="137"/>
+      <c r="K25" s="138"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="139"/>
+      <c r="B26" s="129"/>
+      <c r="C26" s="129"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="129"/>
+      <c r="F26" s="129"/>
+      <c r="G26" s="129"/>
+      <c r="H26" s="129"/>
+      <c r="I26" s="129"/>
+      <c r="J26" s="129"/>
+      <c r="K26" s="140"/>
+    </row>
+    <row r="27" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="144" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="122"/>
-      <c r="C27" s="122"/>
-      <c r="D27" s="122"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="122"/>
-      <c r="G27" s="122"/>
-      <c r="H27" s="122" t="s">
+      <c r="B27" s="145"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="145"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="145"/>
+      <c r="G27" s="145"/>
+      <c r="H27" s="145" t="s">
         <v>117</v>
       </c>
-      <c r="I27" s="122"/>
-      <c r="J27" s="122"/>
-      <c r="K27" s="123"/>
-    </row>
-    <row r="28" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="118" t="s">
+      <c r="I27" s="145"/>
+      <c r="J27" s="145"/>
+      <c r="K27" s="146"/>
+    </row>
+    <row r="28" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="141" t="s">
         <v>116</v>
       </c>
-      <c r="B28" s="119"/>
-      <c r="C28" s="119"/>
-      <c r="D28" s="119"/>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
-      <c r="G28" s="119"/>
-      <c r="H28" s="119" t="s">
+      <c r="B28" s="142"/>
+      <c r="C28" s="142"/>
+      <c r="D28" s="142"/>
+      <c r="E28" s="142"/>
+      <c r="F28" s="142"/>
+      <c r="G28" s="142"/>
+      <c r="H28" s="142" t="s">
         <v>186</v>
       </c>
-      <c r="I28" s="119"/>
-      <c r="J28" s="119"/>
-      <c r="K28" s="120"/>
-    </row>
-    <row r="29" spans="1:15" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I28" s="142"/>
+      <c r="J28" s="142"/>
+      <c r="K28" s="143"/>
+    </row>
+    <row r="29" spans="1:11" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
     </row>
-    <row r="30" spans="1:15" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="124" t="s">
+    <row r="30" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="147" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="125"/>
-      <c r="C30" s="125"/>
-      <c r="D30" s="125"/>
-      <c r="E30" s="125"/>
-      <c r="F30" s="125"/>
-      <c r="G30" s="125"/>
-      <c r="H30" s="125"/>
-      <c r="I30" s="125"/>
-      <c r="J30" s="125"/>
-      <c r="K30" s="126"/>
-      <c r="O30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B30" s="148"/>
+      <c r="C30" s="148"/>
+      <c r="D30" s="148"/>
+      <c r="E30" s="148"/>
+      <c r="F30" s="148"/>
+      <c r="G30" s="148"/>
+      <c r="H30" s="148"/>
+      <c r="I30" s="148"/>
+      <c r="J30" s="148"/>
+      <c r="K30" s="149"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="32" spans="1:11" ht="6.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="127" t="s">
+      <c r="A33" s="150" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="128"/>
-      <c r="C33" s="128"/>
-      <c r="D33" s="128"/>
-      <c r="E33" s="129"/>
-      <c r="F33" s="130"/>
-      <c r="G33" s="130"/>
-      <c r="H33" s="130"/>
+      <c r="B33" s="151"/>
+      <c r="C33" s="151"/>
+      <c r="D33" s="151"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="156"/>
+      <c r="G33" s="156"/>
+      <c r="H33" s="156"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9" t="s">
         <v>12</v>
@@ -10308,18 +10293,18 @@
     </row>
     <row r="34" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="90">
+      <c r="A35" s="153">
         <v>1</v>
       </c>
-      <c r="B35" s="91"/>
-      <c r="C35" s="91"/>
-      <c r="D35" s="91"/>
-      <c r="E35" s="92"/>
-      <c r="F35" s="115" t="s">
-        <v>232</v>
-      </c>
-      <c r="G35" s="116"/>
-      <c r="H35" s="117"/>
+      <c r="B35" s="154"/>
+      <c r="C35" s="154"/>
+      <c r="D35" s="154"/>
+      <c r="E35" s="155"/>
+      <c r="F35" s="106" t="s">
+        <v>231</v>
+      </c>
+      <c r="G35" s="107"/>
+      <c r="H35" s="108"/>
       <c r="I35" s="84">
         <v>1</v>
       </c>
@@ -10329,18 +10314,18 @@
       <c r="K35" s="5"/>
     </row>
     <row r="36" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="90">
+      <c r="A36" s="153">
         <v>2</v>
       </c>
-      <c r="B36" s="91"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="91"/>
-      <c r="E36" s="92"/>
-      <c r="F36" s="115" t="s">
-        <v>233</v>
-      </c>
-      <c r="G36" s="116"/>
-      <c r="H36" s="117"/>
+      <c r="B36" s="154"/>
+      <c r="C36" s="154"/>
+      <c r="D36" s="154"/>
+      <c r="E36" s="155"/>
+      <c r="F36" s="106" t="s">
+        <v>232</v>
+      </c>
+      <c r="G36" s="107"/>
+      <c r="H36" s="108"/>
       <c r="I36" s="84">
         <v>1</v>
       </c>
@@ -10350,18 +10335,18 @@
       <c r="K36" s="5"/>
     </row>
     <row r="37" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="90">
+      <c r="A37" s="153">
         <v>3</v>
       </c>
-      <c r="B37" s="91"/>
-      <c r="C37" s="91"/>
-      <c r="D37" s="91"/>
-      <c r="E37" s="92"/>
-      <c r="F37" s="115" t="s">
-        <v>234</v>
-      </c>
-      <c r="G37" s="116"/>
-      <c r="H37" s="117"/>
+      <c r="B37" s="154"/>
+      <c r="C37" s="154"/>
+      <c r="D37" s="154"/>
+      <c r="E37" s="155"/>
+      <c r="F37" s="106" t="s">
+        <v>233</v>
+      </c>
+      <c r="G37" s="107"/>
+      <c r="H37" s="108"/>
       <c r="I37" s="84">
         <v>1</v>
       </c>
@@ -10371,18 +10356,18 @@
       <c r="K37" s="5"/>
     </row>
     <row r="38" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="90">
+      <c r="A38" s="153">
         <v>4</v>
       </c>
-      <c r="B38" s="91"/>
-      <c r="C38" s="91"/>
-      <c r="D38" s="91"/>
-      <c r="E38" s="92"/>
-      <c r="F38" s="115" t="s">
-        <v>235</v>
-      </c>
-      <c r="G38" s="116"/>
-      <c r="H38" s="117"/>
+      <c r="B38" s="154"/>
+      <c r="C38" s="154"/>
+      <c r="D38" s="154"/>
+      <c r="E38" s="155"/>
+      <c r="F38" s="106" t="s">
+        <v>234</v>
+      </c>
+      <c r="G38" s="107"/>
+      <c r="H38" s="108"/>
       <c r="I38" s="84">
         <v>1</v>
       </c>
@@ -10392,18 +10377,18 @@
       <c r="K38" s="5"/>
     </row>
     <row r="39" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="90">
+      <c r="A39" s="153">
         <v>5</v>
       </c>
-      <c r="B39" s="91"/>
-      <c r="C39" s="91"/>
-      <c r="D39" s="91"/>
-      <c r="E39" s="92"/>
-      <c r="F39" s="115" t="s">
-        <v>236</v>
-      </c>
-      <c r="G39" s="116"/>
-      <c r="H39" s="117"/>
+      <c r="B39" s="154"/>
+      <c r="C39" s="154"/>
+      <c r="D39" s="154"/>
+      <c r="E39" s="155"/>
+      <c r="F39" s="106" t="s">
+        <v>235</v>
+      </c>
+      <c r="G39" s="107"/>
+      <c r="H39" s="108"/>
       <c r="I39" s="84">
         <v>1</v>
       </c>
@@ -10413,18 +10398,18 @@
       <c r="K39" s="5"/>
     </row>
     <row r="40" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="90">
+      <c r="A40" s="153">
         <v>6</v>
       </c>
-      <c r="B40" s="91"/>
-      <c r="C40" s="91"/>
-      <c r="D40" s="91"/>
-      <c r="E40" s="92"/>
-      <c r="F40" s="115" t="s">
-        <v>237</v>
-      </c>
-      <c r="G40" s="116"/>
-      <c r="H40" s="117"/>
+      <c r="B40" s="154"/>
+      <c r="C40" s="154"/>
+      <c r="D40" s="154"/>
+      <c r="E40" s="155"/>
+      <c r="F40" s="106" t="s">
+        <v>236</v>
+      </c>
+      <c r="G40" s="107"/>
+      <c r="H40" s="108"/>
       <c r="I40" s="84">
         <v>1</v>
       </c>
@@ -10434,16 +10419,16 @@
       <c r="K40" s="5"/>
     </row>
     <row r="41" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="90">
+      <c r="A41" s="153">
         <v>7</v>
       </c>
-      <c r="B41" s="91"/>
-      <c r="C41" s="91"/>
-      <c r="D41" s="91"/>
-      <c r="E41" s="92"/>
-      <c r="F41" s="115"/>
-      <c r="G41" s="116"/>
-      <c r="H41" s="117"/>
+      <c r="B41" s="154"/>
+      <c r="C41" s="154"/>
+      <c r="D41" s="154"/>
+      <c r="E41" s="155"/>
+      <c r="F41" s="106"/>
+      <c r="G41" s="107"/>
+      <c r="H41" s="108"/>
       <c r="I41" s="84"/>
       <c r="J41" s="8" t="s">
         <v>118</v>
@@ -10451,16 +10436,16 @@
       <c r="K41" s="5"/>
     </row>
     <row r="42" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="90">
+      <c r="A42" s="153">
         <v>8</v>
       </c>
-      <c r="B42" s="91"/>
-      <c r="C42" s="91"/>
-      <c r="D42" s="91"/>
-      <c r="E42" s="92"/>
-      <c r="F42" s="115"/>
-      <c r="G42" s="116"/>
-      <c r="H42" s="117"/>
+      <c r="B42" s="154"/>
+      <c r="C42" s="154"/>
+      <c r="D42" s="154"/>
+      <c r="E42" s="155"/>
+      <c r="F42" s="106"/>
+      <c r="G42" s="107"/>
+      <c r="H42" s="108"/>
       <c r="I42" s="84"/>
       <c r="J42" s="8" t="s">
         <v>118</v>
@@ -10468,16 +10453,16 @@
       <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="90">
+      <c r="A43" s="153">
         <v>9</v>
       </c>
-      <c r="B43" s="91"/>
-      <c r="C43" s="91"/>
-      <c r="D43" s="91"/>
-      <c r="E43" s="92"/>
-      <c r="F43" s="115"/>
-      <c r="G43" s="116"/>
-      <c r="H43" s="117"/>
+      <c r="B43" s="154"/>
+      <c r="C43" s="154"/>
+      <c r="D43" s="154"/>
+      <c r="E43" s="155"/>
+      <c r="F43" s="106"/>
+      <c r="G43" s="107"/>
+      <c r="H43" s="108"/>
       <c r="I43" s="84"/>
       <c r="J43" s="8" t="s">
         <v>118</v>
@@ -10485,16 +10470,16 @@
       <c r="K43" s="5"/>
     </row>
     <row r="44" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="90">
+      <c r="A44" s="153">
         <v>10</v>
       </c>
-      <c r="B44" s="91"/>
-      <c r="C44" s="91"/>
-      <c r="D44" s="91"/>
-      <c r="E44" s="92"/>
-      <c r="F44" s="115"/>
-      <c r="G44" s="116"/>
-      <c r="H44" s="117"/>
+      <c r="B44" s="154"/>
+      <c r="C44" s="154"/>
+      <c r="D44" s="154"/>
+      <c r="E44" s="155"/>
+      <c r="F44" s="106"/>
+      <c r="G44" s="107"/>
+      <c r="H44" s="108"/>
       <c r="I44" s="84"/>
       <c r="J44" s="8" t="s">
         <v>118</v>
@@ -10502,16 +10487,16 @@
       <c r="K44" s="5"/>
     </row>
     <row r="45" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="90">
+      <c r="A45" s="153">
         <v>11</v>
       </c>
-      <c r="B45" s="91"/>
-      <c r="C45" s="91"/>
-      <c r="D45" s="91"/>
-      <c r="E45" s="92"/>
-      <c r="F45" s="115"/>
-      <c r="G45" s="116"/>
-      <c r="H45" s="117"/>
+      <c r="B45" s="154"/>
+      <c r="C45" s="154"/>
+      <c r="D45" s="154"/>
+      <c r="E45" s="155"/>
+      <c r="F45" s="106"/>
+      <c r="G45" s="107"/>
+      <c r="H45" s="108"/>
       <c r="I45" s="84"/>
       <c r="J45" s="8" t="s">
         <v>118</v>
@@ -10519,16 +10504,16 @@
       <c r="K45" s="5"/>
     </row>
     <row r="46" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="90">
+      <c r="A46" s="153">
         <v>12</v>
       </c>
-      <c r="B46" s="91"/>
-      <c r="C46" s="91"/>
-      <c r="D46" s="91"/>
-      <c r="E46" s="92"/>
-      <c r="F46" s="131"/>
-      <c r="G46" s="131"/>
-      <c r="H46" s="131"/>
+      <c r="B46" s="154"/>
+      <c r="C46" s="154"/>
+      <c r="D46" s="154"/>
+      <c r="E46" s="155"/>
+      <c r="F46" s="110"/>
+      <c r="G46" s="110"/>
+      <c r="H46" s="110"/>
       <c r="I46" s="84"/>
       <c r="J46" s="8" t="s">
         <v>118</v>
@@ -10536,16 +10521,16 @@
       <c r="K46" s="5"/>
     </row>
     <row r="47" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="90">
+      <c r="A47" s="153">
         <v>13</v>
       </c>
-      <c r="B47" s="91"/>
-      <c r="C47" s="91"/>
-      <c r="D47" s="91"/>
-      <c r="E47" s="92"/>
-      <c r="F47" s="131"/>
-      <c r="G47" s="131"/>
-      <c r="H47" s="131"/>
+      <c r="B47" s="154"/>
+      <c r="C47" s="154"/>
+      <c r="D47" s="154"/>
+      <c r="E47" s="155"/>
+      <c r="F47" s="110"/>
+      <c r="G47" s="110"/>
+      <c r="H47" s="110"/>
       <c r="I47" s="81"/>
       <c r="J47" s="8" t="s">
         <v>118</v>
@@ -10553,16 +10538,16 @@
       <c r="K47" s="5"/>
     </row>
     <row r="48" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="90">
+      <c r="A48" s="153">
         <v>14</v>
       </c>
-      <c r="B48" s="91"/>
-      <c r="C48" s="91"/>
-      <c r="D48" s="91"/>
-      <c r="E48" s="92"/>
-      <c r="F48" s="131"/>
-      <c r="G48" s="131"/>
-      <c r="H48" s="131"/>
+      <c r="B48" s="154"/>
+      <c r="C48" s="154"/>
+      <c r="D48" s="154"/>
+      <c r="E48" s="155"/>
+      <c r="F48" s="110"/>
+      <c r="G48" s="110"/>
+      <c r="H48" s="110"/>
       <c r="I48" s="81"/>
       <c r="J48" s="8" t="s">
         <v>118</v>
@@ -10570,16 +10555,16 @@
       <c r="K48" s="5"/>
     </row>
     <row r="49" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="90">
+      <c r="A49" s="153">
         <v>15</v>
       </c>
-      <c r="B49" s="91"/>
-      <c r="C49" s="91"/>
-      <c r="D49" s="91"/>
-      <c r="E49" s="92"/>
-      <c r="F49" s="131"/>
-      <c r="G49" s="131"/>
-      <c r="H49" s="131"/>
+      <c r="B49" s="154"/>
+      <c r="C49" s="154"/>
+      <c r="D49" s="154"/>
+      <c r="E49" s="155"/>
+      <c r="F49" s="110"/>
+      <c r="G49" s="110"/>
+      <c r="H49" s="110"/>
       <c r="I49" s="81"/>
       <c r="J49" s="8" t="s">
         <v>118</v>
@@ -10588,73 +10573,73 @@
     </row>
     <row r="50" spans="1:11" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="25"/>
-      <c r="B50" s="167"/>
-      <c r="C50" s="167"/>
-      <c r="D50" s="167"/>
-      <c r="E50" s="167"/>
-      <c r="F50" s="167"/>
-      <c r="G50" s="167"/>
-      <c r="H50" s="167"/>
+      <c r="B50" s="109"/>
+      <c r="C50" s="109"/>
+      <c r="D50" s="109"/>
+      <c r="E50" s="109"/>
+      <c r="F50" s="109"/>
+      <c r="G50" s="109"/>
+      <c r="H50" s="109"/>
       <c r="I50" s="89"/>
       <c r="J50" s="7"/>
       <c r="K50" s="25"/>
     </row>
     <row r="51" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="168" t="s">
+      <c r="A51" s="111" t="s">
         <v>120</v>
       </c>
-      <c r="B51" s="168"/>
-      <c r="C51" s="168"/>
-      <c r="D51" s="168"/>
-      <c r="E51" s="168"/>
-      <c r="F51" s="168"/>
-      <c r="G51" s="168"/>
-      <c r="H51" s="168"/>
-      <c r="I51" s="168"/>
-      <c r="J51" s="168"/>
-      <c r="K51" s="168"/>
-    </row>
-    <row r="52" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="B51" s="111"/>
+      <c r="C51" s="111"/>
+      <c r="D51" s="111"/>
+      <c r="E51" s="111"/>
+      <c r="F51" s="111"/>
+      <c r="G51" s="111"/>
+      <c r="H51" s="111"/>
+      <c r="I51" s="111"/>
+      <c r="J51" s="111"/>
+      <c r="K51" s="111"/>
+    </row>
+    <row r="52" spans="1:11" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" s="152" t="s">
+      <c r="A53" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="B53" s="153"/>
-      <c r="C53" s="153"/>
-      <c r="D53" s="153"/>
-      <c r="E53" s="153"/>
-      <c r="F53" s="153"/>
-      <c r="G53" s="153"/>
-      <c r="H53" s="153"/>
-      <c r="I53" s="153"/>
-      <c r="J53" s="153"/>
-      <c r="K53" s="154"/>
+      <c r="B53" s="91"/>
+      <c r="C53" s="91"/>
+      <c r="D53" s="91"/>
+      <c r="E53" s="91"/>
+      <c r="F53" s="91"/>
+      <c r="G53" s="91"/>
+      <c r="H53" s="91"/>
+      <c r="I53" s="91"/>
+      <c r="J53" s="91"/>
+      <c r="K53" s="92"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A54" s="155"/>
-      <c r="B54" s="156"/>
-      <c r="C54" s="156"/>
-      <c r="D54" s="156"/>
-      <c r="E54" s="156"/>
-      <c r="F54" s="156"/>
-      <c r="G54" s="156"/>
-      <c r="H54" s="156"/>
-      <c r="I54" s="156"/>
-      <c r="J54" s="156"/>
-      <c r="K54" s="157"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A55" s="158"/>
-      <c r="B55" s="159"/>
-      <c r="C55" s="159"/>
-      <c r="D55" s="159"/>
-      <c r="E55" s="159"/>
-      <c r="F55" s="159"/>
-      <c r="G55" s="159"/>
-      <c r="H55" s="159"/>
-      <c r="I55" s="159"/>
-      <c r="J55" s="159"/>
-      <c r="K55" s="160"/>
+      <c r="A54" s="93"/>
+      <c r="B54" s="94"/>
+      <c r="C54" s="94"/>
+      <c r="D54" s="94"/>
+      <c r="E54" s="94"/>
+      <c r="F54" s="94"/>
+      <c r="G54" s="94"/>
+      <c r="H54" s="94"/>
+      <c r="I54" s="94"/>
+      <c r="J54" s="94"/>
+      <c r="K54" s="95"/>
+    </row>
+    <row r="55" spans="1:11" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="96"/>
+      <c r="B55" s="97"/>
+      <c r="C55" s="97"/>
+      <c r="D55" s="97"/>
+      <c r="E55" s="97"/>
+      <c r="F55" s="97"/>
+      <c r="G55" s="97"/>
+      <c r="H55" s="97"/>
+      <c r="I55" s="97"/>
+      <c r="J55" s="97"/>
+      <c r="K55" s="98"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="86" t="s">
@@ -10673,52 +10658,44 @@
         <v>210</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M97" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>98</v>
       </c>
-      <c r="M99">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="A53:K55"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A6:K7"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A8:G12"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="H23:I23"/>
     <mergeCell ref="F44:H44"/>
     <mergeCell ref="F40:H40"/>
     <mergeCell ref="F41:H41"/>
@@ -10735,44 +10712,41 @@
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A35:E35"/>
     <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A8:G12"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A6:K7"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="A53:K55"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F39:H39"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
-  <colBreaks count="1" manualBreakCount="1">
-    <brk id="11" max="1048575" man="1"/>
-  </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -12519,7 +12493,7 @@
         <v>4551530</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>66</v>
@@ -15288,7 +15262,7 @@
         <v>871345</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>89</v>
@@ -15384,7 +15358,7 @@
         <v>6924637</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>89</v>
@@ -15578,7 +15552,7 @@
         <v>1397233</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C60" s="16" t="s">
         <v>31</v>
@@ -15862,7 +15836,7 @@
         <v>9653692</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C64" s="16" t="s">
         <v>31</v>
@@ -15933,7 +15907,7 @@
         <v>2389734</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C65" s="16" t="s">
         <v>31</v>
@@ -16004,7 +15978,7 @@
         <v>1452832</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C66" s="16" t="s">
         <v>31</v>
@@ -16173,10 +16147,10 @@
         <v>1453037</v>
       </c>
       <c r="B68" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C68" s="16" t="s">
         <v>223</v>
-      </c>
-      <c r="C68" s="16" t="s">
-        <v>224</v>
       </c>
       <c r="D68" s="40" t="s">
         <v>211</v>
@@ -16188,16 +16162,16 @@
         <v>134</v>
       </c>
       <c r="G68" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="H68" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="H68" s="16" t="s">
+      <c r="I68" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="I68" s="16" t="s">
+      <c r="J68" s="16" t="s">
         <v>227</v>
-      </c>
-      <c r="J68" s="16" t="s">
-        <v>228</v>
       </c>
       <c r="K68" s="16" t="s">
         <v>37</v>
@@ -16371,72 +16345,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="133" t="s">
+      <c r="B1" s="113" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
-      <c r="L1" s="135"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="115"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:14" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="136"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="137"/>
-      <c r="L2" s="138"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="118"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="141" t="s">
+      <c r="B3" s="121" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="148"/>
-      <c r="G3" s="148"/>
-      <c r="H3" s="141" t="s">
+      <c r="C3" s="122"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="121" t="s">
         <v>104</v>
       </c>
-      <c r="I3" s="143"/>
-      <c r="J3" s="142"/>
-      <c r="K3" s="147">
+      <c r="I3" s="123"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="127">
         <v>4236654</v>
       </c>
-      <c r="L3" s="188"/>
+      <c r="L3" s="184"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="62"/>
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="142"/>
-      <c r="D4" s="189"/>
-      <c r="E4" s="189"/>
-      <c r="F4" s="189"/>
-      <c r="G4" s="190"/>
-      <c r="H4" s="147" t="s">
+      <c r="C4" s="122"/>
+      <c r="D4" s="180"/>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="181"/>
+      <c r="H4" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="148"/>
+      <c r="I4" s="128"/>
       <c r="J4" s="23"/>
       <c r="K4" s="22" t="s">
         <v>105</v>
@@ -16445,32 +16419,32 @@
     </row>
     <row r="5" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="113" t="s">
+      <c r="B6" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="113"/>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="113"/>
-      <c r="L6" s="113"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="129"/>
+      <c r="L6" s="129"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="113"/>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="113"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="113"/>
-      <c r="L7" s="113"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="129"/>
+      <c r="H7" s="129"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="129"/>
+      <c r="L7" s="129"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="68" t="s">
@@ -16482,14 +16456,14 @@
       <c r="F8" s="68"/>
       <c r="G8" s="68"/>
       <c r="H8" s="68"/>
-      <c r="I8" s="97" t="s">
+      <c r="I8" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="97"/>
-      <c r="K8" s="97" t="s">
+      <c r="J8" s="100"/>
+      <c r="K8" s="100" t="s">
         <v>123</v>
       </c>
-      <c r="L8" s="97"/>
+      <c r="L8" s="100"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="68"/>
@@ -16513,11 +16487,11 @@
       <c r="C10" s="68"/>
       <c r="D10" s="68"/>
       <c r="E10" s="68"/>
-      <c r="F10" s="101" t="s">
+      <c r="F10" s="134" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="102"/>
-      <c r="H10" s="103"/>
+      <c r="G10" s="164"/>
+      <c r="H10" s="135"/>
       <c r="I10" s="46"/>
       <c r="J10" s="36"/>
       <c r="K10" s="4" t="s">
@@ -16530,11 +16504,11 @@
       <c r="C11" s="68"/>
       <c r="D11" s="68"/>
       <c r="E11" s="68"/>
-      <c r="F11" s="101" t="s">
+      <c r="F11" s="134" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="102"/>
-      <c r="H11" s="103"/>
+      <c r="G11" s="164"/>
+      <c r="H11" s="135"/>
       <c r="I11" s="46"/>
       <c r="J11" s="36"/>
       <c r="K11" s="4" t="s">
@@ -16547,11 +16521,11 @@
       <c r="C12" s="68"/>
       <c r="D12" s="68"/>
       <c r="E12" s="68"/>
-      <c r="F12" s="101" t="s">
+      <c r="F12" s="134" t="s">
         <v>106</v>
       </c>
-      <c r="G12" s="102"/>
-      <c r="H12" s="103"/>
+      <c r="G12" s="164"/>
+      <c r="H12" s="135"/>
       <c r="I12" s="24" t="s">
         <v>108</v>
       </c>
@@ -16570,11 +16544,11 @@
       <c r="C13" s="68"/>
       <c r="D13" s="68"/>
       <c r="E13" s="68"/>
-      <c r="F13" s="101" t="s">
+      <c r="F13" s="134" t="s">
         <v>107</v>
       </c>
-      <c r="G13" s="102"/>
-      <c r="H13" s="103"/>
+      <c r="G13" s="164"/>
+      <c r="H13" s="135"/>
       <c r="I13" s="24" t="s">
         <v>108</v>
       </c>
@@ -16602,69 +16576,69 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="98" t="s">
+      <c r="B15" s="161" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="99"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="100"/>
-      <c r="F15" s="101" t="str">
+      <c r="C15" s="162"/>
+      <c r="D15" s="162"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="134" t="str">
         <f>VLOOKUP(K3,Dados!A:H,5,0)</f>
         <v>35 a 50 psi</v>
       </c>
-      <c r="G15" s="102"/>
-      <c r="H15" s="103"/>
-      <c r="I15" s="108" t="s">
+      <c r="G15" s="164"/>
+      <c r="H15" s="135"/>
+      <c r="I15" s="130" t="s">
         <v>121</v>
       </c>
-      <c r="J15" s="108"/>
-      <c r="K15" s="108" t="s">
+      <c r="J15" s="130"/>
+      <c r="K15" s="130" t="s">
         <v>122</v>
       </c>
-      <c r="L15" s="108"/>
+      <c r="L15" s="130"/>
     </row>
     <row r="16" spans="1:14" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="98" t="s">
+      <c r="B16" s="161" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="99"/>
-      <c r="D16" s="99"/>
-      <c r="E16" s="99"/>
-      <c r="F16" s="99"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="105"/>
-      <c r="J16" s="105"/>
-      <c r="K16" s="105"/>
-      <c r="L16" s="106"/>
+      <c r="C16" s="162"/>
+      <c r="D16" s="162"/>
+      <c r="E16" s="162"/>
+      <c r="F16" s="162"/>
+      <c r="G16" s="162"/>
+      <c r="H16" s="162"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
+      <c r="L16" s="167"/>
     </row>
     <row r="17" spans="2:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="104"/>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="105"/>
-      <c r="I17" s="191" t="s">
+      <c r="B17" s="165"/>
+      <c r="C17" s="166"/>
+      <c r="D17" s="166"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="182" t="s">
         <v>187</v>
       </c>
-      <c r="J17" s="192"/>
-      <c r="K17" s="191" t="s">
+      <c r="J17" s="183"/>
+      <c r="K17" s="182" t="s">
         <v>187</v>
       </c>
-      <c r="L17" s="192"/>
+      <c r="L17" s="183"/>
     </row>
     <row r="18" spans="2:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="174" t="s">
+      <c r="B18" s="178" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="132"/>
-      <c r="D18" s="132"/>
-      <c r="E18" s="132"/>
-      <c r="F18" s="132"/>
-      <c r="G18" s="132"/>
-      <c r="H18" s="175"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="185"/>
       <c r="I18" s="39" t="s">
         <v>2</v>
       </c>
@@ -16679,20 +16653,20 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="162" t="s">
+      <c r="B19" s="101" t="s">
         <v>188</v>
       </c>
-      <c r="C19" s="97"/>
-      <c r="D19" s="97"/>
-      <c r="E19" s="97"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="100"/>
       <c r="F19" s="65" t="str">
         <f>VLOOKUP(K3,Dados!A:AF,5,0)</f>
         <v>35 a 50 psi</v>
       </c>
-      <c r="G19" s="97" t="s">
+      <c r="G19" s="100" t="s">
         <v>125</v>
       </c>
-      <c r="H19" s="185"/>
+      <c r="H19" s="173"/>
       <c r="I19" s="54" t="str">
         <f>VLOOKUP(K3,Dados!A:N,14,0)</f>
         <v>____:____</v>
@@ -16711,10 +16685,10 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="176" t="s">
+      <c r="B20" s="186" t="s">
         <v>189</v>
       </c>
-      <c r="C20" s="164"/>
+      <c r="C20" s="103"/>
       <c r="D20" s="67">
         <f>VLOOKUP(K3,Dados!A:O,12,0)</f>
         <v>1</v>
@@ -16726,10 +16700,10 @@
         <f>VLOOKUP(K3,Dados!A:M,13,0)</f>
         <v>N/A</v>
       </c>
-      <c r="G20" s="164" t="s">
+      <c r="G20" s="103" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="200"/>
+      <c r="H20" s="174"/>
       <c r="I20" s="53" t="str">
         <f>VLOOKUP(K3,Dados!A:P,16,0)</f>
         <v>N/A</v>
@@ -16748,58 +16722,58 @@
       </c>
     </row>
     <row r="21" spans="2:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="180" t="s">
+      <c r="B21" s="190" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="181"/>
-      <c r="D21" s="181"/>
-      <c r="E21" s="181"/>
-      <c r="F21" s="132" t="str">
+      <c r="C21" s="191"/>
+      <c r="D21" s="191"/>
+      <c r="E21" s="191"/>
+      <c r="F21" s="112" t="str">
         <f>VLOOKUP(K3,Dados!A:L,6,0)</f>
         <v>15 min./ Mínimo</v>
       </c>
-      <c r="G21" s="132"/>
-      <c r="H21" s="182"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="179"/>
       <c r="I21" s="61"/>
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
       <c r="L21" s="63"/>
     </row>
     <row r="22" spans="2:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="183" t="s">
+      <c r="B22" s="192" t="s">
         <v>112</v>
       </c>
-      <c r="C22" s="184"/>
-      <c r="D22" s="184"/>
-      <c r="E22" s="184"/>
-      <c r="F22" s="97" t="str">
+      <c r="C22" s="193"/>
+      <c r="D22" s="193"/>
+      <c r="E22" s="193"/>
+      <c r="F22" s="100" t="str">
         <f>VLOOKUP(K3,Dados!A:H,8,0)</f>
         <v>120 min./ Mínimo</v>
       </c>
-      <c r="G22" s="97"/>
-      <c r="H22" s="185"/>
+      <c r="G22" s="100"/>
+      <c r="H22" s="173"/>
       <c r="I22" s="52"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="64"/>
     </row>
     <row r="23" spans="2:12" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="186" t="s">
+      <c r="B23" s="194" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="187"/>
-      <c r="D23" s="187"/>
-      <c r="E23" s="187"/>
-      <c r="F23" s="161" t="str">
+      <c r="C23" s="195"/>
+      <c r="D23" s="195"/>
+      <c r="E23" s="195"/>
+      <c r="F23" s="99" t="str">
         <f>VLOOKUP(K3,Dados!A:J,7,0)</f>
         <v>60ºC</v>
       </c>
-      <c r="G23" s="161"/>
-      <c r="H23" s="177"/>
-      <c r="I23" s="196"/>
-      <c r="J23" s="197"/>
-      <c r="K23" s="198"/>
-      <c r="L23" s="199"/>
+      <c r="G23" s="99"/>
+      <c r="H23" s="187"/>
+      <c r="I23" s="169"/>
+      <c r="J23" s="170"/>
+      <c r="K23" s="171"/>
+      <c r="L23" s="172"/>
     </row>
     <row r="24" spans="2:12" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="48"/>
@@ -16815,32 +16789,32 @@
       <c r="L24" s="51"/>
     </row>
     <row r="25" spans="2:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="195"/>
-      <c r="C25" s="195"/>
-      <c r="D25" s="195"/>
-      <c r="E25" s="195"/>
+      <c r="B25" s="177"/>
+      <c r="C25" s="177"/>
+      <c r="D25" s="177"/>
+      <c r="E25" s="177"/>
       <c r="F25" s="50"/>
-      <c r="G25" s="195"/>
-      <c r="H25" s="195"/>
-      <c r="I25" s="193" t="s">
+      <c r="G25" s="177"/>
+      <c r="H25" s="177"/>
+      <c r="I25" s="175" t="s">
         <v>191</v>
       </c>
-      <c r="J25" s="194"/>
-      <c r="K25" s="193" t="s">
+      <c r="J25" s="176"/>
+      <c r="K25" s="175" t="s">
         <v>191</v>
       </c>
-      <c r="L25" s="194"/>
+      <c r="L25" s="176"/>
     </row>
     <row r="26" spans="2:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="174" t="s">
+      <c r="B26" s="178" t="s">
         <v>124</v>
       </c>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
-      <c r="E26" s="132"/>
-      <c r="F26" s="132"/>
-      <c r="G26" s="132"/>
-      <c r="H26" s="182"/>
+      <c r="C26" s="112"/>
+      <c r="D26" s="112"/>
+      <c r="E26" s="112"/>
+      <c r="F26" s="112"/>
+      <c r="G26" s="112"/>
+      <c r="H26" s="179"/>
       <c r="I26" s="59" t="s">
         <v>2</v>
       </c>
@@ -16855,20 +16829,20 @@
       </c>
     </row>
     <row r="27" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="162" t="s">
+      <c r="B27" s="101" t="s">
         <v>188</v>
       </c>
-      <c r="C27" s="97"/>
-      <c r="D27" s="97"/>
-      <c r="E27" s="97"/>
+      <c r="C27" s="100"/>
+      <c r="D27" s="100"/>
+      <c r="E27" s="100"/>
       <c r="F27" s="72">
         <f>VLOOKUP(K3,Dados!A:Y,25,0)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="171" t="s">
+      <c r="G27" s="196" t="s">
         <v>125</v>
       </c>
-      <c r="H27" s="172"/>
+      <c r="H27" s="197"/>
       <c r="I27" s="61">
         <f>VLOOKUP(K3,Dados!A:AE,26,0)</f>
         <v>0</v>
@@ -16887,10 +16861,10 @@
       </c>
     </row>
     <row r="28" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="173" t="s">
+      <c r="B28" s="198" t="s">
         <v>189</v>
       </c>
-      <c r="C28" s="166"/>
+      <c r="C28" s="105"/>
       <c r="D28" s="73">
         <f>VLOOKUP(K3,Dados!A:AE,31,0)</f>
         <v>0</v>
@@ -16902,10 +16876,10 @@
         <f>VLOOKUP(K3,Dados!A:AF,24,0)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="161" t="s">
+      <c r="G28" s="99" t="s">
         <v>126</v>
       </c>
-      <c r="H28" s="177"/>
+      <c r="H28" s="187"/>
       <c r="I28" s="53" t="str">
         <f>VLOOKUP(K3,Dados!A:T,20,0)</f>
         <v>N/A</v>
@@ -16924,139 +16898,139 @@
       </c>
     </row>
     <row r="29" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="93" t="s">
+      <c r="B29" s="157" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="94"/>
-      <c r="D29" s="94"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="178" t="str">
+      <c r="C29" s="158"/>
+      <c r="D29" s="158"/>
+      <c r="E29" s="158"/>
+      <c r="F29" s="188" t="str">
         <f>VLOOKUP(K3,Dados!A:H,6,0)</f>
         <v>15 min./ Mínimo</v>
       </c>
-      <c r="G29" s="178"/>
-      <c r="H29" s="179"/>
+      <c r="G29" s="188"/>
+      <c r="H29" s="189"/>
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
       <c r="K29" s="27"/>
       <c r="L29" s="28"/>
     </row>
     <row r="30" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="98" t="s">
+      <c r="B30" s="161" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="99"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="99"/>
-      <c r="F30" s="102" t="str">
+      <c r="C30" s="162"/>
+      <c r="D30" s="162"/>
+      <c r="E30" s="162"/>
+      <c r="F30" s="164" t="str">
         <f>VLOOKUP(K3,Dados!A:H,8,0)</f>
         <v>120 min./ Mínimo</v>
       </c>
-      <c r="G30" s="102"/>
-      <c r="H30" s="103"/>
+      <c r="G30" s="164"/>
+      <c r="H30" s="135"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="98" t="s">
+      <c r="B31" s="161" t="s">
         <v>113</v>
       </c>
-      <c r="C31" s="99"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="102" t="str">
+      <c r="C31" s="162"/>
+      <c r="D31" s="162"/>
+      <c r="E31" s="162"/>
+      <c r="F31" s="164" t="str">
         <f>VLOOKUP(K3,Dados!A:H,7,0)</f>
         <v>60ºC</v>
       </c>
-      <c r="G31" s="102"/>
-      <c r="H31" s="103"/>
-      <c r="I31" s="95"/>
-      <c r="J31" s="95"/>
-      <c r="K31" s="96"/>
-      <c r="L31" s="96"/>
+      <c r="G31" s="164"/>
+      <c r="H31" s="135"/>
+      <c r="I31" s="159"/>
+      <c r="J31" s="159"/>
+      <c r="K31" s="160"/>
+      <c r="L31" s="160"/>
     </row>
     <row r="32" spans="2:12" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B33" s="109" t="s">
+      <c r="B33" s="136" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="110"/>
-      <c r="D33" s="110"/>
-      <c r="E33" s="110"/>
-      <c r="F33" s="110"/>
-      <c r="G33" s="110"/>
-      <c r="H33" s="110"/>
-      <c r="I33" s="110"/>
-      <c r="J33" s="110"/>
-      <c r="K33" s="110"/>
-      <c r="L33" s="111"/>
+      <c r="C33" s="137"/>
+      <c r="D33" s="137"/>
+      <c r="E33" s="137"/>
+      <c r="F33" s="137"/>
+      <c r="G33" s="137"/>
+      <c r="H33" s="137"/>
+      <c r="I33" s="137"/>
+      <c r="J33" s="137"/>
+      <c r="K33" s="137"/>
+      <c r="L33" s="138"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B34" s="112"/>
-      <c r="C34" s="113"/>
-      <c r="D34" s="113"/>
-      <c r="E34" s="113"/>
-      <c r="F34" s="113"/>
-      <c r="G34" s="113"/>
-      <c r="H34" s="113"/>
-      <c r="I34" s="113"/>
-      <c r="J34" s="113"/>
-      <c r="K34" s="113"/>
-      <c r="L34" s="114"/>
+      <c r="B34" s="139"/>
+      <c r="C34" s="129"/>
+      <c r="D34" s="129"/>
+      <c r="E34" s="129"/>
+      <c r="F34" s="129"/>
+      <c r="G34" s="129"/>
+      <c r="H34" s="129"/>
+      <c r="I34" s="129"/>
+      <c r="J34" s="129"/>
+      <c r="K34" s="129"/>
+      <c r="L34" s="140"/>
     </row>
     <row r="35" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="121" t="s">
+      <c r="B35" s="144" t="s">
         <v>155</v>
       </c>
-      <c r="C35" s="122"/>
-      <c r="D35" s="122"/>
-      <c r="E35" s="122"/>
-      <c r="F35" s="122"/>
-      <c r="G35" s="122"/>
-      <c r="H35" s="122"/>
-      <c r="I35" s="122" t="s">
+      <c r="C35" s="145"/>
+      <c r="D35" s="145"/>
+      <c r="E35" s="145"/>
+      <c r="F35" s="145"/>
+      <c r="G35" s="145"/>
+      <c r="H35" s="145"/>
+      <c r="I35" s="145" t="s">
         <v>117</v>
       </c>
-      <c r="J35" s="122"/>
-      <c r="K35" s="122"/>
-      <c r="L35" s="123"/>
+      <c r="J35" s="145"/>
+      <c r="K35" s="145"/>
+      <c r="L35" s="146"/>
     </row>
     <row r="36" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="118" t="s">
+      <c r="B36" s="141" t="s">
         <v>116</v>
       </c>
-      <c r="C36" s="119"/>
-      <c r="D36" s="119"/>
-      <c r="E36" s="119"/>
-      <c r="F36" s="119"/>
-      <c r="G36" s="119"/>
-      <c r="H36" s="119"/>
-      <c r="I36" s="119" t="s">
+      <c r="C36" s="142"/>
+      <c r="D36" s="142"/>
+      <c r="E36" s="142"/>
+      <c r="F36" s="142"/>
+      <c r="G36" s="142"/>
+      <c r="H36" s="142"/>
+      <c r="I36" s="142" t="s">
         <v>116</v>
       </c>
-      <c r="J36" s="119"/>
-      <c r="K36" s="119"/>
-      <c r="L36" s="120"/>
+      <c r="J36" s="142"/>
+      <c r="K36" s="142"/>
+      <c r="L36" s="143"/>
     </row>
     <row r="37" spans="1:16" ht="3.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="14"/>
     </row>
     <row r="38" spans="1:16" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="124" t="s">
+      <c r="B38" s="147" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="125"/>
-      <c r="D38" s="125"/>
-      <c r="E38" s="125"/>
-      <c r="F38" s="125"/>
-      <c r="G38" s="125"/>
-      <c r="H38" s="125"/>
-      <c r="I38" s="125"/>
-      <c r="J38" s="125"/>
-      <c r="K38" s="125"/>
-      <c r="L38" s="126"/>
+      <c r="C38" s="148"/>
+      <c r="D38" s="148"/>
+      <c r="E38" s="148"/>
+      <c r="F38" s="148"/>
+      <c r="G38" s="148"/>
+      <c r="H38" s="148"/>
+      <c r="I38" s="148"/>
+      <c r="J38" s="148"/>
+      <c r="K38" s="148"/>
+      <c r="L38" s="149"/>
       <c r="P38" t="s">
         <v>16</v>
       </c>
@@ -17071,17 +17045,17 @@
       <c r="B41" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="127" t="s">
+      <c r="C41" s="150" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="128"/>
-      <c r="E41" s="128"/>
-      <c r="F41" s="129"/>
-      <c r="G41" s="130" t="s">
+      <c r="D41" s="151"/>
+      <c r="E41" s="151"/>
+      <c r="F41" s="152"/>
+      <c r="G41" s="156" t="s">
         <v>9</v>
       </c>
-      <c r="H41" s="130"/>
-      <c r="I41" s="130"/>
+      <c r="H41" s="156"/>
+      <c r="I41" s="156"/>
       <c r="J41" s="9" t="s">
         <v>10</v>
       </c>
@@ -17097,17 +17071,17 @@
       <c r="B43" s="5">
         <v>1</v>
       </c>
-      <c r="C43" s="90" t="s">
-        <v>231</v>
-      </c>
-      <c r="D43" s="91"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="92"/>
-      <c r="G43" s="169" t="s">
+      <c r="C43" s="153" t="s">
         <v>230</v>
       </c>
-      <c r="H43" s="169"/>
-      <c r="I43" s="169"/>
+      <c r="D43" s="154"/>
+      <c r="E43" s="154"/>
+      <c r="F43" s="155"/>
+      <c r="G43" s="199" t="s">
+        <v>229</v>
+      </c>
+      <c r="H43" s="199"/>
+      <c r="I43" s="199"/>
       <c r="J43" s="5">
         <v>5</v>
       </c>
@@ -17120,13 +17094,13 @@
       <c r="B44" s="5">
         <v>2</v>
       </c>
-      <c r="C44" s="90"/>
-      <c r="D44" s="91"/>
-      <c r="E44" s="91"/>
-      <c r="F44" s="92"/>
-      <c r="G44" s="169"/>
-      <c r="H44" s="169"/>
-      <c r="I44" s="169"/>
+      <c r="C44" s="153"/>
+      <c r="D44" s="154"/>
+      <c r="E44" s="154"/>
+      <c r="F44" s="155"/>
+      <c r="G44" s="199"/>
+      <c r="H44" s="199"/>
+      <c r="I44" s="199"/>
       <c r="J44" s="5"/>
       <c r="K44" s="8" t="s">
         <v>118</v>
@@ -17137,13 +17111,13 @@
       <c r="B45" s="5">
         <v>3</v>
       </c>
-      <c r="C45" s="90"/>
-      <c r="D45" s="91"/>
-      <c r="E45" s="91"/>
-      <c r="F45" s="92"/>
-      <c r="G45" s="169"/>
-      <c r="H45" s="169"/>
-      <c r="I45" s="169"/>
+      <c r="C45" s="153"/>
+      <c r="D45" s="154"/>
+      <c r="E45" s="154"/>
+      <c r="F45" s="155"/>
+      <c r="G45" s="199"/>
+      <c r="H45" s="199"/>
+      <c r="I45" s="199"/>
       <c r="J45" s="5"/>
       <c r="K45" s="8" t="s">
         <v>118</v>
@@ -17154,13 +17128,13 @@
       <c r="B46" s="5">
         <v>4</v>
       </c>
-      <c r="C46" s="90"/>
-      <c r="D46" s="91"/>
-      <c r="E46" s="91"/>
-      <c r="F46" s="92"/>
-      <c r="G46" s="169"/>
-      <c r="H46" s="169"/>
-      <c r="I46" s="169"/>
+      <c r="C46" s="153"/>
+      <c r="D46" s="154"/>
+      <c r="E46" s="154"/>
+      <c r="F46" s="155"/>
+      <c r="G46" s="199"/>
+      <c r="H46" s="199"/>
+      <c r="I46" s="199"/>
       <c r="J46" s="5"/>
       <c r="K46" s="8" t="s">
         <v>118</v>
@@ -17171,13 +17145,13 @@
       <c r="B47" s="5">
         <v>5</v>
       </c>
-      <c r="C47" s="90"/>
-      <c r="D47" s="91"/>
-      <c r="E47" s="91"/>
-      <c r="F47" s="92"/>
-      <c r="G47" s="169"/>
-      <c r="H47" s="169"/>
-      <c r="I47" s="169"/>
+      <c r="C47" s="153"/>
+      <c r="D47" s="154"/>
+      <c r="E47" s="154"/>
+      <c r="F47" s="155"/>
+      <c r="G47" s="199"/>
+      <c r="H47" s="199"/>
+      <c r="I47" s="199"/>
       <c r="J47" s="5"/>
       <c r="K47" s="8" t="s">
         <v>118</v>
@@ -17188,13 +17162,13 @@
       <c r="B48" s="5">
         <v>6</v>
       </c>
-      <c r="C48" s="90"/>
-      <c r="D48" s="91"/>
-      <c r="E48" s="91"/>
-      <c r="F48" s="92"/>
-      <c r="G48" s="169"/>
-      <c r="H48" s="169"/>
-      <c r="I48" s="169"/>
+      <c r="C48" s="153"/>
+      <c r="D48" s="154"/>
+      <c r="E48" s="154"/>
+      <c r="F48" s="155"/>
+      <c r="G48" s="199"/>
+      <c r="H48" s="199"/>
+      <c r="I48" s="199"/>
       <c r="J48" s="5"/>
       <c r="K48" s="8" t="s">
         <v>118</v>
@@ -17205,13 +17179,13 @@
       <c r="B49" s="5">
         <v>7</v>
       </c>
-      <c r="C49" s="90"/>
-      <c r="D49" s="91"/>
-      <c r="E49" s="91"/>
-      <c r="F49" s="92"/>
-      <c r="G49" s="169"/>
-      <c r="H49" s="169"/>
-      <c r="I49" s="169"/>
+      <c r="C49" s="153"/>
+      <c r="D49" s="154"/>
+      <c r="E49" s="154"/>
+      <c r="F49" s="155"/>
+      <c r="G49" s="199"/>
+      <c r="H49" s="199"/>
+      <c r="I49" s="199"/>
       <c r="J49" s="5"/>
       <c r="K49" s="8" t="s">
         <v>118</v>
@@ -17222,13 +17196,13 @@
       <c r="B50" s="5">
         <v>8</v>
       </c>
-      <c r="C50" s="90"/>
-      <c r="D50" s="91"/>
-      <c r="E50" s="91"/>
-      <c r="F50" s="92"/>
-      <c r="G50" s="169"/>
-      <c r="H50" s="169"/>
-      <c r="I50" s="169"/>
+      <c r="C50" s="153"/>
+      <c r="D50" s="154"/>
+      <c r="E50" s="154"/>
+      <c r="F50" s="155"/>
+      <c r="G50" s="199"/>
+      <c r="H50" s="199"/>
+      <c r="I50" s="199"/>
       <c r="J50" s="6"/>
       <c r="K50" s="8" t="s">
         <v>118</v>
@@ -17239,13 +17213,13 @@
       <c r="B51" s="5">
         <v>9</v>
       </c>
-      <c r="C51" s="90"/>
-      <c r="D51" s="91"/>
-      <c r="E51" s="91"/>
-      <c r="F51" s="92"/>
-      <c r="G51" s="169"/>
-      <c r="H51" s="169"/>
-      <c r="I51" s="169"/>
+      <c r="C51" s="153"/>
+      <c r="D51" s="154"/>
+      <c r="E51" s="154"/>
+      <c r="F51" s="155"/>
+      <c r="G51" s="199"/>
+      <c r="H51" s="199"/>
+      <c r="I51" s="199"/>
       <c r="J51" s="6"/>
       <c r="K51" s="8" t="s">
         <v>118</v>
@@ -17256,13 +17230,13 @@
       <c r="B52" s="5">
         <v>10</v>
       </c>
-      <c r="C52" s="90"/>
-      <c r="D52" s="91"/>
-      <c r="E52" s="91"/>
-      <c r="F52" s="92"/>
-      <c r="G52" s="169"/>
-      <c r="H52" s="169"/>
-      <c r="I52" s="169"/>
+      <c r="C52" s="153"/>
+      <c r="D52" s="154"/>
+      <c r="E52" s="154"/>
+      <c r="F52" s="155"/>
+      <c r="G52" s="199"/>
+      <c r="H52" s="199"/>
+      <c r="I52" s="199"/>
       <c r="J52" s="6"/>
       <c r="K52" s="8" t="s">
         <v>118</v>
@@ -17271,84 +17245,84 @@
     </row>
     <row r="53" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="25"/>
-      <c r="C53" s="167"/>
-      <c r="D53" s="167"/>
-      <c r="E53" s="167"/>
-      <c r="F53" s="167"/>
-      <c r="G53" s="167"/>
-      <c r="H53" s="167"/>
-      <c r="I53" s="167"/>
+      <c r="C53" s="109"/>
+      <c r="D53" s="109"/>
+      <c r="E53" s="109"/>
+      <c r="F53" s="109"/>
+      <c r="G53" s="109"/>
+      <c r="H53" s="109"/>
+      <c r="I53" s="109"/>
       <c r="K53" s="7"/>
       <c r="L53" s="25"/>
     </row>
     <row r="54" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="168" t="s">
+      <c r="B54" s="111" t="s">
         <v>120</v>
       </c>
-      <c r="C54" s="168"/>
-      <c r="D54" s="168"/>
-      <c r="E54" s="168"/>
-      <c r="F54" s="168"/>
-      <c r="G54" s="168"/>
-      <c r="H54" s="168"/>
-      <c r="I54" s="168"/>
-      <c r="J54" s="168"/>
-      <c r="K54" s="168"/>
-      <c r="L54" s="168"/>
+      <c r="C54" s="111"/>
+      <c r="D54" s="111"/>
+      <c r="E54" s="111"/>
+      <c r="F54" s="111"/>
+      <c r="G54" s="111"/>
+      <c r="H54" s="111"/>
+      <c r="I54" s="111"/>
+      <c r="J54" s="111"/>
+      <c r="K54" s="111"/>
+      <c r="L54" s="111"/>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B56" s="170" t="s">
+      <c r="B56" s="200" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="170"/>
-      <c r="D56" s="170"/>
-      <c r="E56" s="170"/>
-      <c r="F56" s="170"/>
-      <c r="G56" s="170"/>
-      <c r="H56" s="170"/>
-      <c r="I56" s="170"/>
-      <c r="J56" s="170"/>
-      <c r="K56" s="170"/>
-      <c r="L56" s="170"/>
+      <c r="C56" s="200"/>
+      <c r="D56" s="200"/>
+      <c r="E56" s="200"/>
+      <c r="F56" s="200"/>
+      <c r="G56" s="200"/>
+      <c r="H56" s="200"/>
+      <c r="I56" s="200"/>
+      <c r="J56" s="200"/>
+      <c r="K56" s="200"/>
+      <c r="L56" s="200"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B57" s="170"/>
-      <c r="C57" s="170"/>
-      <c r="D57" s="170"/>
-      <c r="E57" s="170"/>
-      <c r="F57" s="170"/>
-      <c r="G57" s="170"/>
-      <c r="H57" s="170"/>
-      <c r="I57" s="170"/>
-      <c r="J57" s="170"/>
-      <c r="K57" s="170"/>
-      <c r="L57" s="170"/>
+      <c r="B57" s="200"/>
+      <c r="C57" s="200"/>
+      <c r="D57" s="200"/>
+      <c r="E57" s="200"/>
+      <c r="F57" s="200"/>
+      <c r="G57" s="200"/>
+      <c r="H57" s="200"/>
+      <c r="I57" s="200"/>
+      <c r="J57" s="200"/>
+      <c r="K57" s="200"/>
+      <c r="L57" s="200"/>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B58" s="170"/>
-      <c r="C58" s="170"/>
-      <c r="D58" s="170"/>
-      <c r="E58" s="170"/>
-      <c r="F58" s="170"/>
-      <c r="G58" s="170"/>
-      <c r="H58" s="170"/>
-      <c r="I58" s="170"/>
-      <c r="J58" s="170"/>
-      <c r="K58" s="170"/>
-      <c r="L58" s="170"/>
+      <c r="B58" s="200"/>
+      <c r="C58" s="200"/>
+      <c r="D58" s="200"/>
+      <c r="E58" s="200"/>
+      <c r="F58" s="200"/>
+      <c r="G58" s="200"/>
+      <c r="H58" s="200"/>
+      <c r="I58" s="200"/>
+      <c r="J58" s="200"/>
+      <c r="K58" s="200"/>
+      <c r="L58" s="200"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B59" s="170"/>
-      <c r="C59" s="170"/>
-      <c r="D59" s="170"/>
-      <c r="E59" s="170"/>
-      <c r="F59" s="170"/>
-      <c r="G59" s="170"/>
-      <c r="H59" s="170"/>
-      <c r="I59" s="170"/>
-      <c r="J59" s="170"/>
-      <c r="K59" s="170"/>
-      <c r="L59" s="170"/>
+      <c r="B59" s="200"/>
+      <c r="C59" s="200"/>
+      <c r="D59" s="200"/>
+      <c r="E59" s="200"/>
+      <c r="F59" s="200"/>
+      <c r="G59" s="200"/>
+      <c r="H59" s="200"/>
+      <c r="I59" s="200"/>
+      <c r="J59" s="200"/>
+      <c r="K59" s="200"/>
+      <c r="L59" s="200"/>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
@@ -17360,55 +17334,26 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B6:L7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="B16:L16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B1:L2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="C52:F52"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="B56:L59"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="B54:L54"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="C46:F46"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="G47:I47"/>
     <mergeCell ref="C44:F44"/>
     <mergeCell ref="G44:I44"/>
     <mergeCell ref="I31:J31"/>
@@ -17425,26 +17370,55 @@
     <mergeCell ref="G41:I41"/>
     <mergeCell ref="C43:F43"/>
     <mergeCell ref="G43:I43"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="C52:F52"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="B56:L59"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="B54:L54"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="B1:L2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B6:L7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="B16:L16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>

</xml_diff>